<commit_message>
changes in upload functionality
</commit_message>
<xml_diff>
--- a/public/file/book.xlsx
+++ b/public/file/book.xlsx
@@ -1,32 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D78A7909-A964-4894-B359-627D249D7290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\try\Marketer\public\file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA9E23C-56A1-4116-8256-ECCC38F1649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>client_name</t>
   </si>
@@ -50,13 +44,37 @@
   </si>
   <si>
     <t>sikarwaraman26@gmail.com</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>customer_type</t>
+  </si>
+  <si>
+    <t>Rishabh</t>
+  </si>
+  <si>
+    <t>rishwebd@gmail.com</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>1234-567-890</t>
+  </si>
+  <si>
+    <t>B2B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,51 +430,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{248EC45F-61E2-4C13-985A-BB056F19C822}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{6863A07D-A465-46F7-B7ED-F7B20920E6D8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{F63D3B32-0E09-40F1-8AC8-101FDA981F78}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{248EC45F-61E2-4C13-985A-BB056F19C822}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{6863A07D-A465-46F7-B7ED-F7B20920E6D8}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{F63D3B32-0E09-40F1-8AC8-101FDA981F78}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{12321823-35E7-47DC-A9CF-68730AE5D500}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>